<commit_message>
Student Profile Page Updated
</commit_message>
<xml_diff>
--- a/media/student/Student Data.xlsx
+++ b/media/student/Student Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOME\Desktop\TSG-Hackathon\media\student\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B8AB5F-A814-4BDE-9D2C-E8EADB6CC19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BECF94B-6F94-4A89-A17F-BC5802F0DFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="996" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,7 +89,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -107,12 +107,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -133,9 +127,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -144,10 +137,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -367,7 +359,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -454,9 +446,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" xr:uid="{2BF60619-2DCB-46F7-AC42-DA5E7DF238AF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>